<commit_message>
Update 251020_홍콩 KTU 3단계 진행 일정 및 결과1.xlsx
</commit_message>
<xml_diff>
--- a/251020_홍콩 KTU 3단계 진행 일정 및 결과1.xlsx
+++ b/251020_홍콩 KTU 3단계 진행 일정 및 결과1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\1_BEUPSYS\4_계약진행\2_현대로템\4_PO\250930_KTU신역사방송소프트웨어업데이트\2_일정\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/JDS_BU/Git_Hub/GIC_HONGKONG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC570857-273F-47AC-A38A-08F150F2BEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D205078-C5EB-B448-A8D2-F9783CE89F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grace AI 수행" sheetId="4" r:id="rId1"/>
@@ -30,15 +30,12 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>월</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -242,6 +239,10 @@
   </si>
   <si>
     <t>외주</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>888888ㅗ8ㅗ8</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -816,6 +817,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -831,6 +835,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -851,12 +858,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1256,20 +1257,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08D818E-D923-4937-BD18-3B9C91A5DAD8}">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="17.600000000000001"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="10.640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="21" customWidth="1"/>
     <col min="5" max="18" width="3.5" style="21" customWidth="1"/>
-    <col min="19" max="16384" width="8.640625" style="21"/>
+    <col min="19" max="16384" width="8.6640625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -1282,46 +1283,46 @@
     </row>
     <row r="2" spans="1:18" ht="18" thickBot="1"/>
     <row r="3" spans="1:18">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45" t="s">
+      <c r="F3" s="46"/>
+      <c r="G3" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45" t="s">
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45" t="s">
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="47"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="22" t="s">
         <v>29</v>
       </c>
@@ -1390,7 +1391,7 @@
       <c r="R5" s="42"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="47" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="23" t="s">
@@ -1414,7 +1415,7 @@
       <c r="R6" s="27"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="46"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="23" t="s">
         <v>35</v>
       </c>
@@ -1436,7 +1437,7 @@
       <c r="R7" s="27"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="46"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="23" t="s">
         <v>36</v>
       </c>
@@ -1458,7 +1459,7 @@
       <c r="R8" s="26"/>
     </row>
     <row r="9" spans="1:18" ht="30">
-      <c r="A9" s="46"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23" t="s">
         <v>48</v>
@@ -1482,7 +1483,7 @@
       <c r="R9" s="26"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="46"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23" t="s">
         <v>47</v>
@@ -1504,7 +1505,7 @@
       <c r="R10" s="26"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="46"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="23" t="s">
         <v>37</v>
       </c>
@@ -1526,7 +1527,7 @@
       <c r="R11" s="26"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="46"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="29" t="s">
         <v>38</v>
       </c>
@@ -1548,7 +1549,7 @@
       <c r="R12" s="26"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="46"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="23" t="s">
         <v>39</v>
       </c>
@@ -1581,7 +1582,7 @@
       <c r="E14" s="39"/>
       <c r="F14" s="39"/>
       <c r="G14" s="39"/>
-      <c r="H14" s="58"/>
+      <c r="H14" s="45"/>
       <c r="I14" s="40"/>
       <c r="J14" s="40"/>
       <c r="K14" s="40"/>
@@ -1617,7 +1618,7 @@
       <c r="Q15" s="27"/>
       <c r="R15" s="27"/>
     </row>
-    <row r="16" spans="1:18" ht="18" thickBot="1">
+    <row r="16" spans="1:18" ht="31" thickBot="1">
       <c r="A16" s="33" t="s">
         <v>42</v>
       </c>
@@ -1660,6 +1661,11 @@
       <c r="P17" s="38"/>
       <c r="Q17" s="38"/>
       <c r="R17" s="38"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="B20" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1686,59 +1692,59 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.600000000000001"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="2" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="47.5703125" customWidth="1"/>
-    <col min="5" max="7" width="2.2109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="9" max="13" width="2.2109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.5" customWidth="1"/>
+    <col min="5" max="7" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" customWidth="1"/>
+    <col min="9" max="13" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="20" width="3" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="35.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="18" thickBot="1"/>
     <row r="2" spans="2:21" s="1" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="52" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="55" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="55" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="55" t="s">
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="53" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="55" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:21" s="1" customFormat="1" ht="17.25" customHeight="1">
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1790,13 +1796,13 @@
       <c r="T3" s="6">
         <v>16</v>
       </c>
-      <c r="U3" s="54"/>
-    </row>
-    <row r="4" spans="2:21" s="1" customFormat="1" ht="53.15" customHeight="1">
-      <c r="B4" s="52" t="s">
+      <c r="U3" s="56"/>
+    </row>
+    <row r="4" spans="2:21" s="1" customFormat="1" ht="53.25" customHeight="1">
+      <c r="B4" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="54" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -1821,8 +1827,8 @@
       <c r="U4" s="14"/>
     </row>
     <row r="5" spans="2:21" s="1" customFormat="1" ht="42" customHeight="1">
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="19" t="s">
         <v>9</v>
       </c>
@@ -1845,8 +1851,8 @@
       <c r="U5" s="15"/>
     </row>
     <row r="6" spans="2:21" s="1" customFormat="1" ht="37" customHeight="1">
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="19" t="s">
         <v>10</v>
       </c>
@@ -1869,8 +1875,8 @@
       <c r="U6" s="15"/>
     </row>
     <row r="7" spans="2:21" s="1" customFormat="1" ht="34" customHeight="1">
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="19" t="s">
         <v>11</v>
       </c>
@@ -1892,9 +1898,9 @@
       <c r="T7" s="11"/>
       <c r="U7" s="15"/>
     </row>
-    <row r="8" spans="2:21" s="1" customFormat="1" ht="38.15" customHeight="1">
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
+    <row r="8" spans="2:21" s="1" customFormat="1" ht="38.25" customHeight="1">
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="19" t="s">
         <v>12</v>
       </c>
@@ -1916,9 +1922,9 @@
       <c r="T8" s="11"/>
       <c r="U8" s="15"/>
     </row>
-    <row r="9" spans="2:21" s="1" customFormat="1" ht="38.15" customHeight="1">
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
+    <row r="9" spans="2:21" s="1" customFormat="1" ht="38.25" customHeight="1">
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="19" t="s">
         <v>13</v>
       </c>

</xml_diff>